<commit_message>
organizational changes, edits to abstracts, minor script tweaks, clonal stock count data
</commit_message>
<xml_diff>
--- a/data/stock_tracker.xlsx
+++ b/data/stock_tracker.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\timet\Documents\projectCSUN\csunThesisRepo\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8312DD0E-CF70-440B-A99E-D14AF42E4B66}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A9BE466-7C17-4C56-81F8-A346379BC13C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{3D4B1669-294A-4F20-BCA3-8F8B2599EBA8}"/>
+    <workbookView xWindow="2355" yWindow="1050" windowWidth="22200" windowHeight="14100" xr2:uid="{3D4B1669-294A-4F20-BCA3-8F8B2599EBA8}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -87,15 +87,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -435,7 +435,7 @@
   <dimension ref="A1:E19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+      <selection activeCell="C25" sqref="C25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -444,22 +444,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="C1" s="4"/>
-      <c r="D1" s="4"/>
-      <c r="E1" s="4"/>
+      <c r="C1" s="5"/>
+      <c r="D1" s="5"/>
+      <c r="E1" s="5"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="2"/>
-      <c r="B2" s="3" t="s">
+      <c r="A2" s="3"/>
+      <c r="B2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="2" t="s">
         <v>0</v>
       </c>
       <c r="D2" t="s">
@@ -480,9 +480,12 @@
         <f>B3/0.3</f>
         <v>103.33333333333334</v>
       </c>
+      <c r="D3">
+        <v>13</v>
+      </c>
       <c r="E3" s="1">
         <f>D3/0.3</f>
-        <v>0</v>
+        <v>43.333333333333336</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
@@ -496,9 +499,12 @@
         <f t="shared" ref="C4:E19" si="0">B4/0.3</f>
         <v>93.333333333333343</v>
       </c>
+      <c r="D4">
+        <v>20</v>
+      </c>
       <c r="E4" s="1">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>66.666666666666671</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
@@ -512,9 +518,12 @@
         <f t="shared" si="0"/>
         <v>153.33333333333334</v>
       </c>
+      <c r="D5">
+        <v>18</v>
+      </c>
       <c r="E5" s="1">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>60</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
@@ -528,9 +537,12 @@
         <f t="shared" si="0"/>
         <v>113.33333333333334</v>
       </c>
+      <c r="D6">
+        <v>8</v>
+      </c>
       <c r="E6" s="1">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>26.666666666666668</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
@@ -544,9 +556,12 @@
         <f t="shared" si="0"/>
         <v>43.333333333333336</v>
       </c>
+      <c r="D7">
+        <v>22</v>
+      </c>
       <c r="E7" s="1">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>73.333333333333343</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
@@ -560,9 +575,12 @@
         <f t="shared" si="0"/>
         <v>20</v>
       </c>
+      <c r="D8">
+        <v>8</v>
+      </c>
       <c r="E8" s="1">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>26.666666666666668</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
@@ -576,9 +594,12 @@
         <f t="shared" si="0"/>
         <v>66.666666666666671</v>
       </c>
+      <c r="D9">
+        <v>25</v>
+      </c>
       <c r="E9" s="1">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>83.333333333333343</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
@@ -592,9 +613,12 @@
         <f t="shared" si="0"/>
         <v>86.666666666666671</v>
       </c>
+      <c r="D10">
+        <v>57</v>
+      </c>
       <c r="E10" s="1">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>190</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
@@ -608,9 +632,12 @@
         <f t="shared" si="0"/>
         <v>73.333333333333343</v>
       </c>
+      <c r="D11">
+        <v>8</v>
+      </c>
       <c r="E11" s="1">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>26.666666666666668</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
@@ -624,9 +651,12 @@
         <f t="shared" si="0"/>
         <v>113.33333333333334</v>
       </c>
+      <c r="D12">
+        <v>24</v>
+      </c>
       <c r="E12" s="1">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>80</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
@@ -640,9 +670,12 @@
         <f t="shared" si="0"/>
         <v>110</v>
       </c>
+      <c r="D13">
+        <v>23</v>
+      </c>
       <c r="E13" s="1">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>76.666666666666671</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
@@ -656,9 +689,12 @@
         <f t="shared" si="0"/>
         <v>20</v>
       </c>
+      <c r="D14">
+        <v>14</v>
+      </c>
       <c r="E14" s="1">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>46.666666666666671</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
@@ -672,9 +708,12 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
+      <c r="D15">
+        <v>1</v>
+      </c>
       <c r="E15" s="1">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>3.3333333333333335</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
@@ -688,9 +727,12 @@
         <f t="shared" si="0"/>
         <v>13.333333333333334</v>
       </c>
+      <c r="D16">
+        <v>3</v>
+      </c>
       <c r="E16" s="1">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>10</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
@@ -704,9 +746,12 @@
         <f t="shared" si="0"/>
         <v>50</v>
       </c>
+      <c r="D17">
+        <v>11</v>
+      </c>
       <c r="E17" s="1">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>36.666666666666671</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
@@ -720,9 +765,12 @@
         <f t="shared" si="0"/>
         <v>93.333333333333343</v>
       </c>
+      <c r="D18">
+        <v>25</v>
+      </c>
       <c r="E18" s="1">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>83.333333333333343</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
@@ -736,9 +784,12 @@
         <f t="shared" si="0"/>
         <v>113.33333333333334</v>
       </c>
+      <c r="D19">
+        <v>20</v>
+      </c>
       <c r="E19" s="1">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>66.666666666666671</v>
       </c>
     </row>
   </sheetData>

</xml_diff>